<commit_message>
Fix 2 cases where one phrase was split into two
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - Latein - Fachvokabular Jus - Multiple Choice (JKU, Austria).xlsx
+++ b/flashcards/Memcode - Latein - Fachvokabular Jus - Multiple Choice (JKU, Austria).xlsx
@@ -19,6 +19,36 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;&lt;strong&gt;praes, praedis m.:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verlegung des Gerichtsstandes&lt;/li&gt;&lt;li&gt;ein einmal erloschener Anspruch lebt nicht wieder auf&lt;/li&gt;&lt;li&gt;Verschiedenheit&lt;/li&gt;&lt;li&gt;Bürge&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Bürge&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;iura praediorum urbanorum:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rechte an städtischen Grundstücken oder Gebäudeservituten&lt;/li&gt;&lt;li&gt;Recht des Anbietens und Nachfolgens&lt;/li&gt;&lt;li&gt;eine Person, die bereits zur Ausführung einer Tat entschlossen ist&lt;/li&gt;&lt;li&gt;die Mutter ist immer gewiss&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Rechte an städtischen Grundstücken oder Gebäudeservituten</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;arbitrium iudicis:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Schwere, Gewicht, Last&lt;/li&gt;&lt;li&gt;Absicht, Wille (des Handelnden)&lt;/li&gt;&lt;li&gt;richterliches Ermessen&lt;/li&gt;&lt;li&gt;der Richter möge nicht über das Begehren der Parteien hinausgehen &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>richterliches Ermessen</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;uno actu:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;in einem Akt&lt;/li&gt;&lt;li&gt;die Abtretung vor Gericht (Eigentumsübertragungsform des römischen Rechts)&lt;/li&gt;&lt;li&gt;der Richter möge nicht über das Begehren der Parteien hinausgehen &lt;/li&gt;&lt;li&gt;römisches Staatsamt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>in einem Akt</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;ne eat iudex ultra petita patrium:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gesetzbuch, Gesetzessammlung&lt;/li&gt;&lt;li&gt;der Richter möge nicht über das Begehren der Parteien hinausgehen&lt;/li&gt;&lt;li&gt;einjahrig befristetes Klagerecht&lt;/li&gt;&lt;li&gt;Rechtsnachfolge, Erbfolge&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;der Richter möge nicht über das Begehren der Parteien hinausgehen&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;&lt;strong&gt;quod licet Iovi non licet bovi:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Forderungsabtretung&lt;/li&gt;&lt;li&gt;eigenberechtigte Person&lt;/li&gt;&lt;li&gt;zum Schein&lt;/li&gt;&lt;li&gt;was Jupiter erlaubt ist, ist dem Ochsen nicht erlaubt (Ausdruck unterschiedlicher persönlicher Freiheiten nach Status)&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
@@ -73,7 +103,7 @@
     <t>Wort, Aussage</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong&gt;onus, -eris n. pl.: onera:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Last, Leistung, Beschwer&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;onus, -eris n. pl.: onera:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Last, Leistung, Beschwerde&lt;/li&gt;&lt;li&gt;Verkürzung über die Hälfte („übermäßig große“ Verletzung)&lt;/li&gt;&lt;li&gt;Schlussfolgerung vom Größeren auf das Kleine&lt;/li&gt;&lt;li&gt;einer Tat entschlossen sein&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>Last, Leistung, Beschwer</t>
@@ -1222,12 +1252,6 @@
   </si>
   <si>
     <t>Vorschrift, Verjährung</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;b&gt;praes, praedis m.:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verlegung des Gerichtsstandes&lt;/li&gt;&lt;li&gt;ein einmal erloschener Anspruch lebt nicht wieder auf&lt;/li&gt;&lt;li&gt;Verschiedenheit&lt;/li&gt;&lt;li&gt;Burge&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>Burge</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;b&gt;praedium, -i n.:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verurteilung&lt;/li&gt;&lt;li&gt;Ursache, (Rechts)grund, Titel
@@ -1625,16 +1649,16 @@
     <t>jede Definition im bürgerlichen Recht ist gefährlich</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;omnis definitio in iure civile:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gesellschafter (vgl heute „Sozius“)&lt;/li&gt;&lt;li&gt;töten&lt;/li&gt;&lt;li&gt;Miteigentum&lt;/li&gt;&lt;li&gt;einer Tat entschlossen ist&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>einer Tat entschlossen ist</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;b&gt;omni modo facturus:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Klage aus der Geschäftsführung ohne Auftrag&lt;/li&gt;&lt;li&gt;Schutzherr / Herr&lt;/li&gt;&lt;li&gt;Unterscheidung im Recht&lt;/li&gt;&lt;li&gt;eine Person, die bereits zur Ausführung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>eine Person, die bereits zur Ausführung</t>
+    <t>&lt;p&gt;&lt;strong&gt;omnis definitio in iure civile periculosa est:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gesellschafter (vgl heute „Sozius“)&lt;/li&gt;&lt;li&gt;töten&lt;/li&gt;&lt;li&gt;Miteigentum&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;jede Definition im bürgerlichen Recht ist gefährlich&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;jede Definition im bürgerlichen Recht ist gefährlich&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;omni modo facturus:&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Klage aus der Geschäftsführung ohne Auftrag&lt;/li&gt;&lt;li&gt;Schutzherr / Herr&lt;/li&gt;&lt;li&gt;Unterscheidung im Recht&lt;/li&gt;&lt;li&gt;eine Person, die bereits zur Ausführung einer Tat entschlossen ist &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;eine Person, die bereits zur Ausführung einer Tat entschlossen ist&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;b&gt;odium, -i n.:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Hass&lt;/li&gt;&lt;li&gt;nach dem Tod&lt;/li&gt;&lt;li&gt;Verbannung, Exil&lt;/li&gt;&lt;li&gt;Hauptanklage, direkte Klage des Hauptanspruchsberechtigten&lt;/li&gt;&lt;/ul&gt;</t>
@@ -1984,12 +2008,6 @@
   </si>
   <si>
     <t>Stadt</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;b&gt;uno actu:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;in einem Akt&lt;/li&gt;&lt;li&gt;die Abtretung vor Gericht (Eigentumsübertragungsform des römischen Rechts)&lt;/li&gt;&lt;li&gt;der Richter möge nicht über das Begehren der Parteien hinausgehen hinausgehen&lt;/li&gt;&lt;li&gt;römisches Staatsamt&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>in einem Akt</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;b&gt;universitas, -atis f.:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;der Ort bestimmt das Geschehen&lt;/li&gt;&lt;li&gt;(Personen-)Gesamtheit, Körperschaft&lt;/li&gt;&lt;li&gt;Ursprung&lt;/li&gt;&lt;li&gt;öffentliche Bekanntmachung&lt;/li&gt;&lt;/ul&gt;</t>
@@ -2435,12 +2453,6 @@
     <t>die Notwendigkeit hat kein Gesetz</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;b&gt;ne eat iudex ultra petita patrium:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Gesetzbuch, Gesetzessammlung&lt;/li&gt;&lt;li&gt;der Richter möge nicht über das Begehren der Parteien hinausgehen hinausgehen&lt;/li&gt;&lt;li&gt;einjahrig befristetes Klagerecht&lt;/li&gt;&lt;li&gt;Rechtsnachfolge, Erbfolge&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>der Richter möge nicht über das Begehren der Parteien hinausgehen hinausgehen</t>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;b&gt;naturalis possessio:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Anklage&lt;/li&gt;&lt;li&gt;die (durch Beischlaf) vollzogene Ehe&lt;/li&gt;&lt;li&gt;für die Öffentlichkeit bestimmt&lt;/li&gt;&lt;li&gt;natürlicher Besitz&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
@@ -3141,12 +3153,6 @@
   </si>
   <si>
     <t>niemand ist verpflichtet, von dem ihm zustehenden Recht Gebrauch zu machen</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;b&gt;iura praediorum urbanorum:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rechte an städtischen Grundstücken oder Gebäudeservituten&lt;/li&gt;&lt;li&gt;Recht des Anbietens und Nachfolgens&lt;/li&gt;&lt;li&gt;eine Person, die bereits zur Ausführung&lt;/li&gt;&lt;li&gt;die Mutter ist immer gewiss&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>Rechte an städtischen Grundstücken oder Gebäudeservituten</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;b&gt;dolus directus:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Preis, Wert, „Zins“&lt;/li&gt;&lt;li&gt;letzter Wille&lt;/li&gt;&lt;li&gt;direkter Vorsatz&lt;/li&gt;&lt;li&gt;Gegenstand des Verbrechens / Beweisstück&lt;/li&gt;&lt;/ul&gt;</t>
@@ -5726,12 +5732,6 @@
   </si>
   <si>
     <t>Schiedsspruch</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;b&gt;arbitrium iudicis:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Schwere, Gewicht, Last&lt;/li&gt;&lt;li&gt;Absicht, Wille (des Handelnden)&lt;/li&gt;&lt;li&gt;richterliches Ermessen&lt;/li&gt;&lt;li&gt;der Richter möge nicht über das Begehren der Parteien hinausgehen hinausgehen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>richterliches Ermessen</t>
   </si>
   <si>
     <t>&lt;p&gt;&lt;b&gt;approbatio, -ionis f.:&lt;/b&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rechtsunkenntnis&lt;/li&gt;&lt;li&gt;durch Gewahrsam und Besitzwillen&lt;/li&gt;&lt;li&gt;Bestätigung, Billigung&lt;/li&gt;&lt;li&gt;auf einem Vertrage beruhend&lt;/li&gt;&lt;/ul&gt;</t>
@@ -7763,47 +7763,47 @@
         <v>198</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>169</v>
+        <v>199</v>
       </c>
     </row>
     <row r="101" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
     </row>
     <row r="103" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="105" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>208</v>
+        <v>179</v>
       </c>
     </row>
     <row r="106" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -10075,31 +10075,31 @@
         <v>775</v>
       </c>
       <c r="B389" s="2" t="s">
-        <v>726</v>
+        <v>776</v>
       </c>
     </row>
     <row r="390" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A390" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="B390" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
     </row>
     <row r="391" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A391" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="B391" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
     </row>
     <row r="392" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A392" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="B392" s="2" t="s">
-        <v>781</v>
+        <v>732</v>
       </c>
     </row>
     <row r="393" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -12099,15 +12099,15 @@
         <v>1280</v>
       </c>
       <c r="B642" s="2" t="s">
-        <v>1153</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="643" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A643" s="2" t="s">
-        <v>1281</v>
+        <v>1282</v>
       </c>
       <c r="B643" s="2" t="s">
-        <v>1282</v>
+        <v>1155</v>
       </c>
     </row>
     <row r="644" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -15075,7 +15075,7 @@
         <v>2023</v>
       </c>
       <c r="B1014" s="2" t="s">
-        <v>330</v>
+        <v>340</v>
       </c>
     </row>
     <row r="1015" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>